<commit_message>
Finalized schematic V1.0; minor changes to symbol library
</commit_message>
<xml_diff>
--- a/Hardware/BAT_Materialliste.xlsx
+++ b/Hardware/BAT_Materialliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\Module\TA.BA_BAA+E.F2401\Entwicklung\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4268752A-7864-4417-A18A-3CF214B9B168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC60092-F30D-429C-A599-E95AD784764C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>Hersteller</t>
   </si>
@@ -576,7 +576,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,6 +669,9 @@
       </c>
       <c r="E4">
         <v>4.5890000000000004</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>